<commit_message>
update source code for Verilog thesis traffic light
</commit_message>
<xml_diff>
--- a/Verilog/Thesis_FPGA_Traffic_Light/output_file/Phan_tich.xlsx
+++ b/Verilog/Thesis_FPGA_Traffic_Light/output_file/Phan_tich.xlsx
@@ -12292,11 +12292,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="133989792"/>
-        <c:axId val="378192992"/>
+        <c:axId val="319797136"/>
+        <c:axId val="319798704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133989792"/>
+        <c:axId val="319797136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12356,7 +12356,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378192992"/>
+        <c:crossAx val="319798704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12364,7 +12364,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="378192992"/>
+        <c:axId val="319798704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12425,7 +12425,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133989792"/>
+        <c:crossAx val="319797136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -30428,7 +30428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>